<commit_message>
add synthea test data for connectathon
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386B163F-A7D5-4AA1-90FA-8F13D22CF912}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7309C45-7F14-422B-A6C7-15066F490B52}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="2715" windowWidth="18900" windowHeight="11055" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19935" yWindow="1260" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -1599,9 +1599,6 @@
  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.argo-3.1.0</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-pulse-oximetry</t>
   </si>
   <si>
@@ -1729,6 +1726,9 @@
   </si>
   <si>
     <t>Fetches an AllergyIntolerance resource  (within the clients authorization scope) and any corresponding Provenance resources.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core-3.1.0</t>
   </si>
 </sst>
 </file>
@@ -2212,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2251,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>482</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2668,10 +2668,10 @@
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>484</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -2710,16 +2710,16 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -2733,7 +2733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2957,7 +2957,7 @@
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1" ht="15">
       <c r="A22" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
@@ -3199,7 +3199,7 @@
         <v>422</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -6792,7 +6792,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -6893,7 +6893,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -6995,7 +6995,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -7048,7 +7048,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -7106,7 +7106,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>
@@ -8892,7 +8892,7 @@
         <v>21</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>73</v>
@@ -8911,15 +8911,15 @@
         <v>60</v>
       </c>
       <c r="I95" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y95" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y95" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z95" s="7"/>
       <c r="AA95" s="12"/>
       <c r="AB95" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="96" spans="1:28" ht="18.95" customHeight="1">
@@ -8930,7 +8930,7 @@
         <v>248</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>73</v>
@@ -8949,15 +8949,15 @@
         <v>60</v>
       </c>
       <c r="I96" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y96" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y96" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z96" s="7"/>
       <c r="AA96" s="12"/>
       <c r="AB96" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="18.95" customHeight="1">
@@ -8968,7 +8968,7 @@
         <v>262</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>73</v>
@@ -8987,15 +8987,15 @@
         <v>60</v>
       </c>
       <c r="I97" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y97" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y97" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z97" s="7"/>
       <c r="AA97" s="12"/>
       <c r="AB97" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="18.95" customHeight="1">
@@ -9006,7 +9006,7 @@
         <v>143</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>73</v>
@@ -9025,15 +9025,15 @@
         <v>60</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y98" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y98" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z98" s="7"/>
       <c r="AA98" s="12"/>
       <c r="AB98" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="18.95" customHeight="1">
@@ -9044,7 +9044,7 @@
         <v>187</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>73</v>
@@ -9063,15 +9063,15 @@
         <v>60</v>
       </c>
       <c r="I99" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y99" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y99" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z99" s="7"/>
       <c r="AA99" s="12"/>
       <c r="AB99" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="18.95" customHeight="1">
@@ -9082,7 +9082,7 @@
         <v>186</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>73</v>
@@ -9101,15 +9101,15 @@
         <v>60</v>
       </c>
       <c r="I100" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y100" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y100" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z100" s="7"/>
       <c r="AA100" s="12"/>
       <c r="AB100" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="18.95" customHeight="1">
@@ -9120,7 +9120,7 @@
         <v>23</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>73</v>
@@ -9139,15 +9139,15 @@
         <v>60</v>
       </c>
       <c r="I101" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y101" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y101" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z101" s="7"/>
       <c r="AA101" s="12"/>
       <c r="AB101" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="18.95" customHeight="1">
@@ -9158,7 +9158,7 @@
         <v>188</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>73</v>
@@ -9177,15 +9177,15 @@
         <v>60</v>
       </c>
       <c r="I102" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y102" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y102" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z102" s="7"/>
       <c r="AA102" s="12"/>
       <c r="AB102" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="18.95" customHeight="1">
@@ -9196,7 +9196,7 @@
         <v>167</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>73</v>
@@ -9215,15 +9215,15 @@
         <v>60</v>
       </c>
       <c r="I103" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y103" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y103" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z103" s="7"/>
       <c r="AA103" s="12"/>
       <c r="AB103" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="18.95" customHeight="1">
@@ -9234,7 +9234,7 @@
         <v>266</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>73</v>
@@ -9253,15 +9253,15 @@
         <v>60</v>
       </c>
       <c r="I104" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y104" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y104" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z104" s="7"/>
       <c r="AA104" s="12"/>
       <c r="AB104" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="18.95" customHeight="1">
@@ -9272,7 +9272,7 @@
         <v>191</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>73</v>
@@ -9291,15 +9291,15 @@
         <v>60</v>
       </c>
       <c r="I105" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y105" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y105" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z105" s="7"/>
       <c r="AA105" s="12"/>
       <c r="AB105" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="18.95" customHeight="1">
@@ -9310,7 +9310,7 @@
         <v>267</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>73</v>
@@ -9329,15 +9329,15 @@
         <v>60</v>
       </c>
       <c r="I106" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y106" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y106" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z106" s="7"/>
       <c r="AA106" s="12"/>
       <c r="AB106" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="18.95" customHeight="1">
@@ -9348,7 +9348,7 @@
         <v>389</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>73</v>
@@ -9367,15 +9367,15 @@
         <v>60</v>
       </c>
       <c r="I107" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y107" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y107" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z107" s="7"/>
       <c r="AA107" s="12"/>
       <c r="AB107" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="18.95" customHeight="1">
@@ -9386,7 +9386,7 @@
         <v>189</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>73</v>
@@ -9405,15 +9405,15 @@
         <v>60</v>
       </c>
       <c r="I108" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y108" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y108" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z108" s="7"/>
       <c r="AA108" s="12"/>
       <c r="AB108" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="18.95" customHeight="1">
@@ -9424,7 +9424,7 @@
         <v>281</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>73</v>
@@ -9443,15 +9443,15 @@
         <v>60</v>
       </c>
       <c r="I109" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y109" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y109" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z109" s="7"/>
       <c r="AA109" s="12"/>
       <c r="AB109" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="18.95" customHeight="1">
@@ -9462,7 +9462,7 @@
         <v>22</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>73</v>
@@ -9481,15 +9481,15 @@
         <v>60</v>
       </c>
       <c r="I110" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y110" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y110" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z110" s="7"/>
       <c r="AA110" s="12"/>
       <c r="AB110" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="18.95" customHeight="1">
@@ -9500,7 +9500,7 @@
         <v>288</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>73</v>
@@ -9519,15 +9519,15 @@
         <v>60</v>
       </c>
       <c r="I111" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y111" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y111" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z111" s="7"/>
       <c r="AA111" s="12"/>
       <c r="AB111" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="18.95" customHeight="1">
@@ -9538,7 +9538,7 @@
         <v>291</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>73</v>
@@ -9557,15 +9557,15 @@
         <v>60</v>
       </c>
       <c r="I112" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y112" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y112" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z112" s="7"/>
       <c r="AA112" s="12"/>
       <c r="AB112" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="18.95" customHeight="1">
@@ -9576,7 +9576,7 @@
         <v>190</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>73</v>
@@ -9595,15 +9595,15 @@
         <v>60</v>
       </c>
       <c r="I113" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y113" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y113" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z113" s="7"/>
       <c r="AA113" s="12"/>
       <c r="AB113" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -10168,13 +10168,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H20" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B20&amp;"s and associated provenance for a patient")</f>
@@ -10201,13 +10201,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H21" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B21&amp;" and its associated provenance")</f>
@@ -10591,13 +10591,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H35" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B35&amp;"s and associated provenance for a patient")</f>
@@ -10624,13 +10624,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H36" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B36&amp;" and its associated provenance")</f>
@@ -10780,13 +10780,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H41" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B41&amp;"s and associated provenance for a patient")</f>
@@ -10813,13 +10813,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H42" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B42&amp;" and its associated provenance")</f>
@@ -10861,7 +10861,7 @@
         <v>351</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -10876,22 +10876,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D44" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="H44" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="J44" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -10906,22 +10906,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D45" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="H45" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -10998,13 +10998,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H48" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B48&amp;"s and associated provenance for a patient")</f>
@@ -11031,13 +11031,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H49" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B49&amp;" and its associated provenance")</f>
@@ -11219,13 +11219,13 @@
         <v>197</v>
       </c>
       <c r="D55" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H55" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B55&amp;"s and associated provenance for a patient")</f>
@@ -11251,13 +11251,13 @@
         <v>197</v>
       </c>
       <c r="D56" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H56" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B56&amp;" and its associated provenance")</f>
@@ -11433,13 +11433,13 @@
         <v>198</v>
       </c>
       <c r="D62" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H62" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B62&amp;"s and associated provenance for a patient")</f>
@@ -11465,13 +11465,13 @@
         <v>198</v>
       </c>
       <c r="D63" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H63" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B63&amp;" and its associated provenance")</f>
@@ -11560,13 +11560,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D66" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H66" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B66&amp;"s and associated provenance for a patient")</f>
@@ -11593,13 +11593,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D67" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H67" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B67&amp;" and its associated provenance")</f>
@@ -11626,7 +11626,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>73</v>
@@ -11635,16 +11635,16 @@
         <v>111</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="H68" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -11659,7 +11659,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>73</v>
@@ -11668,7 +11668,7 @@
         <v>111</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>194</v>
@@ -11677,7 +11677,7 @@
         <v>460</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -11692,7 +11692,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>73</v>
@@ -11701,7 +11701,7 @@
         <v>111</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>194</v>
@@ -11710,7 +11710,7 @@
         <v>460</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -11725,7 +11725,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>73</v>
@@ -11734,7 +11734,7 @@
         <v>229</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>244</v>
@@ -11743,7 +11743,7 @@
         <v>461</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -11758,13 +11758,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D72" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H72" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B72&amp;"s and associated provenance for a patient")</f>
@@ -11791,13 +11791,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D73" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H73" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B73&amp;" and its associated provenance")</f>
@@ -11817,7 +11817,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11848,7 +11848,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11978,13 +11978,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D79" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H79" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B79&amp;"s and associated provenance for a patient")</f>
@@ -12011,13 +12011,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D80" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H80" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B80&amp;" and its associated provenance")</f>
@@ -12052,13 +12052,13 @@
         <v>111</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J81" s="5" t="s">
         <v>347</v>
@@ -12084,13 +12084,13 @@
         <v>111</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12147,13 +12147,13 @@
         <v>229</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J84" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12231,13 +12231,13 @@
         <v>451</v>
       </c>
       <c r="D87" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H87" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B87&amp;"s and associated provenance for a patient")</f>
@@ -12263,13 +12263,13 @@
         <v>451</v>
       </c>
       <c r="D88" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H88" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B88&amp;" and its associated provenance")</f>
@@ -12425,13 +12425,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="D93" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H93" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B93&amp;"s and associated provenance for a patient")</f>
@@ -12458,13 +12458,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="D94" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H94" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B94&amp;" and its associated provenance")</f>
@@ -12524,13 +12524,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D96" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H96" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B96&amp;"s and associated provenance for a patient")</f>
@@ -12557,13 +12557,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D97" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H97" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B97&amp;" and its associated provenance")</f>
@@ -12622,13 +12622,13 @@
         <v>297</v>
       </c>
       <c r="D99" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H99" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B99&amp;"s and associated provenance for a patient")</f>
@@ -12654,13 +12654,13 @@
         <v>297</v>
       </c>
       <c r="D100" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H100" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B100&amp;" and its associated provenance")</f>
@@ -12695,13 +12695,13 @@
         <v>111</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J101" s="5" t="str">
         <f t="shared" ref="J101" si="9">"Fetches a bundle of all "&amp;B101&amp;" resources for the specified "&amp;SUBSTITUTE(D101,","," and ")</f>
@@ -12728,13 +12728,13 @@
         <v>111</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>300</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J102" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -12761,7 +12761,7 @@
         <v>111</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>303</v>
@@ -12794,13 +12794,13 @@
         <v>229</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H104" s="5" t="s">
         <v>306</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J104" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -12848,13 +12848,13 @@
         <v>345</v>
       </c>
       <c r="D106" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H106" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B106&amp;"s and associated provenance for a patient")</f>
@@ -12880,13 +12880,13 @@
         <v>345</v>
       </c>
       <c r="D107" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H107" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B107&amp;" and its associated provenance")</f>
@@ -13100,13 +13100,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D114" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H114" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B114&amp;"s and associated provenance for a patient")</f>
@@ -13133,13 +13133,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D115" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H115" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B115&amp;" and its associated provenance")</f>
@@ -13194,13 +13194,13 @@
         <v>475</v>
       </c>
       <c r="D117" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H117" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B117&amp;"s and associated provenance for a patient")</f>
@@ -13226,13 +13226,13 @@
         <v>475</v>
       </c>
       <c r="D118" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H118" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B118&amp;" and its associated provenance")</f>
@@ -13258,13 +13258,13 @@
         <v>475</v>
       </c>
       <c r="D119" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H119" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B119&amp;"s and associated provenance for a patient")</f>
@@ -13290,13 +13290,13 @@
         <v>475</v>
       </c>
       <c r="D120" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H120" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B120&amp;" and its associated provenance")</f>
@@ -13322,13 +13322,13 @@
         <v>475</v>
       </c>
       <c r="D121" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F121" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H121" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B121&amp;"s and associated provenance for a patient")</f>
@@ -13354,13 +13354,13 @@
         <v>475</v>
       </c>
       <c r="D122" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H122" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B122&amp;" and its associated provenance")</f>
@@ -13386,13 +13386,13 @@
         <v>475</v>
       </c>
       <c r="D123" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F123" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H123" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B123&amp;"s and associated provenance for a patient")</f>
@@ -13418,13 +13418,13 @@
         <v>475</v>
       </c>
       <c r="D124" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H124" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B124&amp;" and its associated provenance")</f>
@@ -13450,13 +13450,13 @@
         <v>475</v>
       </c>
       <c r="D125" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F125" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H125" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B125&amp;"s and associated provenance for a patient")</f>
@@ -13482,13 +13482,13 @@
         <v>475</v>
       </c>
       <c r="D126" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H126" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B126&amp;" and its associated provenance")</f>

</xml_diff>